<commit_message>
Added a new project that implements a QR Code processor based upon ZXing.Net. Migrated existing xUnit test projects from the Tardigrade Framework Solution to a new Solution. Updated NuGet packages.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafRafiq\Source\tardigrade-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94506C8-1BA8-403E-A91D-8453E0F5736F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122D88E-740D-443B-A63E-2DA7DCDC8FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10644" yWindow="3696" windowWidth="18156" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52" yWindow="0" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -109,13 +109,49 @@
   </si>
   <si>
     <t>1.2.3</t>
+  </si>
+  <si>
+    <t>10.5.0</t>
+  </si>
+  <si>
+    <t>8.8.0</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>3.2.3</t>
+  </si>
+  <si>
+    <t>1.2.1</t>
+  </si>
+  <si>
+    <t>5.3.2</t>
+  </si>
+  <si>
+    <t>9.2.1</t>
+  </si>
+  <si>
+    <t>8.1.2</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Tardigrade.Framework.ZXingNet</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,14 +161,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -162,8 +190,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,29 +472,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -476,30 +507,39 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -509,19 +549,25 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -531,38 +577,64 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
General enhancements and code clean-up.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122D88E-740D-443B-A63E-2DA7DCDC8FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE3B5B-89A6-4086-9161-C5BC8C71A356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52" yWindow="0" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4673" yWindow="2355" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -145,6 +145,33 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>9.0.0</t>
+  </si>
+  <si>
+    <t>11.0.0</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>3.3.0</t>
+  </si>
+  <si>
+    <t>1.3.0</t>
+  </si>
+  <si>
+    <t>9.3.0</t>
+  </si>
+  <si>
+    <t>8.2.0</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>6.0.0</t>
   </si>
 </sst>
 </file>
@@ -472,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -483,7 +510,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -496,8 +523,11 @@
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -510,8 +540,11 @@
       <c r="D2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -524,8 +557,11 @@
       <c r="D3" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -538,8 +574,11 @@
       <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -552,8 +591,11 @@
       <c r="D5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -566,8 +608,11 @@
       <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -580,8 +625,11 @@
       <c r="D7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -594,8 +642,11 @@
       <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E8" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -608,8 +659,11 @@
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -622,8 +676,11 @@
       <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -635,6 +692,9 @@
       </c>
       <c r="D11" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted changes to the Create operations of the Repository class in the EntityFrameworkCore project that rejected object IDs set to their "default" values.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE3B5B-89A6-4086-9161-C5BC8C71A356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148E287C-2A2A-42BA-BC2B-14082827C348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4673" yWindow="2355" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6488" yWindow="3255" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>6.0.0</t>
+  </si>
+  <si>
+    <t>11.1.0</t>
+  </si>
+  <si>
+    <t>8.3.0</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -510,7 +516,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -526,8 +532,11 @@
       <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +553,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -560,8 +569,9 @@
       <c r="E3" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -577,8 +587,9 @@
       <c r="E4" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -595,7 +606,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -611,8 +622,9 @@
       <c r="E6" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -629,7 +641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -645,8 +657,11 @@
       <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -662,8 +677,9 @@
       <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -679,8 +695,9 @@
       <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -696,6 +713,7 @@
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Replaced usage of "GetAwaiter().GetResult()" with "AsyncHelper.RunSync(() => asyncMethod())" in the AzureStorage project due to upgrade issues moving to the Microsoft.Azure.Cosmos.Table NuGet package.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148E287C-2A2A-42BA-BC2B-14082827C348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5739F6B-B114-4672-9D3A-007D0D837BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6488" yWindow="3255" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>8.3.0</t>
+  </si>
+  <si>
+    <t>11.2.0</t>
+  </si>
+  <si>
+    <t>6.1.0</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -516,7 +522,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -535,8 +541,11 @@
       <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -553,7 +562,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -570,8 +579,9 @@
         <v>42</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -588,8 +598,9 @@
         <v>43</v>
       </c>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -606,7 +617,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -623,8 +634,11 @@
         <v>48</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -641,7 +655,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -660,8 +674,9 @@
       <c r="F8" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -678,8 +693,9 @@
         <v>44</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -696,8 +712,9 @@
         <v>43</v>
       </c>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -714,6 +731,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated IdentityUserManager implementations to include a DeleteAsync() method.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5739F6B-B114-4672-9D3A-007D0D837BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577AAC7-3EDF-4FBF-A976-6ADA42524F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6488" yWindow="3255" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4133" yWindow="2490" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -184,6 +184,39 @@
   </si>
   <si>
     <t>6.1.0</t>
+  </si>
+  <si>
+    <t>11.3.0</t>
+  </si>
+  <si>
+    <t>9.1.0</t>
+  </si>
+  <si>
+    <t>5.1.0</t>
+  </si>
+  <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
+  </si>
+  <si>
+    <t>9.3.1</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>6.1.1</t>
+  </si>
+  <si>
+    <t>8.3.1</t>
   </si>
 </sst>
 </file>
@@ -511,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -522,7 +555,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -544,8 +577,11 @@
       <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -561,8 +597,11 @@
       <c r="E2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -580,8 +619,11 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -599,8 +641,11 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -616,8 +661,11 @@
       <c r="E5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -637,8 +685,11 @@
       <c r="G6" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -654,8 +705,11 @@
       <c r="E7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -675,8 +729,11 @@
         <v>50</v>
       </c>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -694,8 +751,11 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -713,8 +773,11 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -732,6 +795,9 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhanced the Repository layer to handle derived types from a class hierarchy.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577AAC7-3EDF-4FBF-A976-6ADA42524F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD3BE13-7B46-4B9B-920D-387C82FECF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4133" yWindow="2490" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="1808" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>8.3.1</t>
+  </si>
+  <si>
+    <t>11.4.0</t>
+  </si>
+  <si>
+    <t>10.0.0</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -555,7 +561,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -580,8 +586,11 @@
       <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -601,7 +610,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -622,8 +631,9 @@
       <c r="H3" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -644,8 +654,9 @@
       <c r="H4" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -665,7 +676,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -688,8 +699,9 @@
       <c r="H6" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -708,8 +720,11 @@
       <c r="H7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -732,8 +747,9 @@
       <c r="H8" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -754,8 +770,9 @@
       <c r="H9" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -776,8 +793,9 @@
       <c r="H10" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -798,6 +816,7 @@
       <c r="H11" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated third-party NuGet packages. Updated version numbers of all Tardigrade packages.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD3BE13-7B46-4B9B-920D-387C82FECF85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E13D0-00FE-4584-862D-5576DBC64804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="1808" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -223,13 +223,43 @@
   </si>
   <si>
     <t>10.0.0</t>
+  </si>
+  <si>
+    <t>11.5.0</t>
+  </si>
+  <si>
+    <t>2.1.0</t>
+  </si>
+  <si>
+    <t>5.1.1</t>
+  </si>
+  <si>
+    <t>8.3.2</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>6.1.2</t>
+  </si>
+  <si>
+    <t>10.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +269,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -266,10 +304,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -561,7 +600,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -589,8 +628,11 @@
       <c r="I1" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J1" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -609,8 +651,11 @@
       <c r="H2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -632,8 +677,11 @@
         <v>55</v>
       </c>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J3" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -655,8 +703,11 @@
         <v>56</v>
       </c>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -675,8 +726,11 @@
       <c r="H5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -700,8 +754,11 @@
         <v>62</v>
       </c>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J6" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -723,8 +780,11 @@
       <c r="I7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J7" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -748,8 +808,11 @@
         <v>63</v>
       </c>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J8" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -771,8 +834,11 @@
         <v>59</v>
       </c>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J9" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -794,8 +860,11 @@
         <v>60</v>
       </c>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J10" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -817,6 +886,9 @@
         <v>61</v>
       </c>
       <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Redesigned the IRepository interface so that it no longer extends the IBulkRepository interface. Instead implementing classes need to implement IBulkRepository explicitly.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09E13D0-00FE-4584-862D-5576DBC64804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138DF9B8-5B11-405F-B27F-D690A64D9867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3278" yWindow="3278" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -225,18 +225,12 @@
     <t>10.0.0</t>
   </si>
   <si>
-    <t>11.5.0</t>
-  </si>
-  <si>
     <t>2.1.0</t>
   </si>
   <si>
     <t>5.1.1</t>
   </si>
   <si>
-    <t>8.3.2</t>
-  </si>
-  <si>
     <t>3.4.1</t>
   </si>
   <si>
@@ -249,10 +243,13 @@
     <t>1.1.2</t>
   </si>
   <si>
-    <t>6.1.2</t>
-  </si>
-  <si>
     <t>10.0.1</t>
+  </si>
+  <si>
+    <t>7.0.0</t>
+  </si>
+  <si>
+    <t>12.0.0</t>
   </si>
 </sst>
 </file>
@@ -592,7 +589,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -629,7 +626,7 @@
         <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -652,7 +649,7 @@
         <v>54</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -678,7 +675,7 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -704,7 +701,7 @@
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -727,7 +724,7 @@
         <v>57</v>
       </c>
       <c r="J5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
@@ -754,8 +751,8 @@
         <v>62</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="3" t="s">
-        <v>74</v>
+      <c r="J6" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -781,7 +778,7 @@
         <v>65</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
@@ -809,7 +806,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
@@ -835,7 +832,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
@@ -861,7 +858,7 @@
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
@@ -887,7 +884,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed the Repository classes of the AzureStorage project to remove the "AzureStorage" prefix.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138DF9B8-5B11-405F-B27F-D690A64D9867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1ED679-1BAF-4ACE-80C0-DE17F6FFC4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3278" yWindow="3278" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,13 +243,13 @@
     <t>1.1.2</t>
   </si>
   <si>
-    <t>10.0.1</t>
-  </si>
-  <si>
     <t>7.0.0</t>
   </si>
   <si>
     <t>12.0.0</t>
+  </si>
+  <si>
+    <t>10.1.0</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -626,7 +626,7 @@
         <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
@@ -752,7 +752,7 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -777,8 +777,8 @@
       <c r="I7" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>72</v>
+      <c r="J7" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Removed a redundant generic parameter from the IDtoService interface.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1ED679-1BAF-4ACE-80C0-DE17F6FFC4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB1BD54-E41F-4C56-9BB3-95FDF48D56EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3278" yWindow="3278" windowWidth="21599" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added classes for managing application configuration settings. Created unit tests for these classes. Updated NuGet packages.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB1BD54-E41F-4C56-9BB3-95FDF48D56EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370295C5-ED7A-4F6A-8A26-0C0302E1786F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -250,6 +250,15 @@
   </si>
   <si>
     <t>10.1.0</t>
+  </si>
+  <si>
+    <t>12.1.0</t>
+  </si>
+  <si>
+    <t>3.4.2</t>
+  </si>
+  <si>
+    <t>9.0.1</t>
   </si>
 </sst>
 </file>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -597,7 +606,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -628,8 +637,11 @@
       <c r="J1" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -651,8 +663,11 @@
       <c r="J2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -677,8 +692,9 @@
       <c r="J3" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -703,8 +719,11 @@
       <c r="J4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -727,7 +746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -754,8 +773,9 @@
       <c r="J6" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -780,8 +800,9 @@
       <c r="J7" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -808,8 +829,11 @@
       <c r="J8" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -834,8 +858,9 @@
       <c r="J9" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -860,8 +885,9 @@
       <c r="J10" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -886,6 +912,7 @@
       <c r="J11" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Moved the IdentityUserDbContext class from the EntityFramework project to the AspNet project.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370295C5-ED7A-4F6A-8A26-0C0302E1786F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D3275-E97A-4B8C-9209-E24344FAD2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5805" yWindow="3645" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>9.0.1</t>
+  </si>
+  <si>
+    <t>5.2.0</t>
   </si>
 </sst>
 </file>
@@ -598,7 +601,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -692,7 +695,9 @@
       <c r="J3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -800,7 +805,9 @@
       <c r="J7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Enhanced ApplicationManager to support database application settings.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capta\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D3275-E97A-4B8C-9209-E24344FAD2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F4D20B-574D-4723-94E9-10ABDECDD6E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="3645" windowWidth="21600" windowHeight="11423" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>5.2.0</t>
+  </si>
+  <si>
+    <t>13.0.0</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
   </si>
 </sst>
 </file>
@@ -598,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -609,7 +615,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -643,8 +649,11 @@
       <c r="K1" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -669,8 +678,11 @@
       <c r="K2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -698,8 +710,9 @@
       <c r="K3" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -727,8 +740,11 @@
       <c r="K4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -751,7 +767,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -779,8 +795,9 @@
         <v>72</v>
       </c>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -808,8 +825,11 @@
       <c r="K7" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -839,8 +859,11 @@
       <c r="K8" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L8" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -866,8 +889,9 @@
         <v>69</v>
       </c>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -893,8 +917,9 @@
         <v>70</v>
       </c>
       <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -920,6 +945,7 @@
         <v>71</v>
       </c>
       <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhanced ConfigurationExtension to support more type casting options.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capta\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F4D20B-574D-4723-94E9-10ABDECDD6E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F1F4D-5E24-40FA-9864-CE1BAF30AD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="4080" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>4.0.0</t>
+  </si>
+  <si>
+    <t>13.1.0</t>
   </si>
 </sst>
 </file>
@@ -604,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -615,7 +618,7 @@
     <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -652,8 +655,11 @@
       <c r="L1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -681,8 +687,11 @@
       <c r="L2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -712,7 +721,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -744,7 +753,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -767,7 +776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -797,7 +806,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -829,7 +838,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -863,7 +872,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -891,7 +900,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -919,7 +928,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Updated documentation ready for release.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capta\Source\tardigrade-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F1F4D-5E24-40FA-9864-CE1BAF30AD20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C2BD2D-8737-413A-90F4-2383F355D1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="4080" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1347" yWindow="1573" windowWidth="22306" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>13.1.0</t>
+  </si>
+  <si>
+    <t>14.0.0</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>8.0.0</t>
+  </si>
+  <si>
+    <t>Tardigrade.Framework.MailKit</t>
   </si>
 </sst>
 </file>
@@ -607,18 +619,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="38.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.52734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -658,8 +671,11 @@
       <c r="M1" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -690,8 +706,11 @@
       <c r="M2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -720,8 +739,11 @@
         <v>78</v>
       </c>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -752,8 +774,11 @@
       <c r="L4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -775,8 +800,11 @@
       <c r="J5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -805,8 +833,11 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -837,8 +868,11 @@
       <c r="L7" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -871,90 +905,120 @@
       <c r="L8" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>44</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
+      <c r="N11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="N12" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhanced the ToEnum<T>(string) and ToEnum<T>(string, T) methods of the EnumExtension class to cater for the Display attribute.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C2BD2D-8737-413A-90F4-2383F355D1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4B186E-59D2-4A4A-950B-1AF44A4DC613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1347" yWindow="1573" windowWidth="22306" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="487" yWindow="3393" windowWidth="22306" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Tardigrade.Framework.MailKit</t>
+  </si>
+  <si>
+    <t>14.1.0</t>
   </si>
 </sst>
 </file>
@@ -619,11 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A10" sqref="A10"/>
+      <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -631,7 +634,7 @@
     <col min="1" max="1" width="38.52734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -674,8 +677,11 @@
       <c r="N1" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="O1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -709,8 +715,11 @@
       <c r="N2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+      <c r="O2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -743,7 +752,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -778,7 +787,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -804,7 +813,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -837,7 +846,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -872,7 +881,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -909,25 +918,51 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="N9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -958,7 +993,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -989,7 +1024,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
- Renamed the DisplayName property of the EmailAddress class to Name. - Consolidated .NET Standard-style projects to support .NET 6 where appropriate.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4B186E-59D2-4A4A-950B-1AF44A4DC613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438A738-780C-40C4-B417-C1F3BF3F7837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="487" yWindow="3393" windowWidth="22306" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="99">
   <si>
     <t>Tardigrade.Framework</t>
   </si>
@@ -286,6 +287,42 @@
   </si>
   <si>
     <t>14.1.0</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>AspNet</t>
+  </si>
+  <si>
+    <t>AspNetCore</t>
+  </si>
+  <si>
+    <t>AuditNET</t>
+  </si>
+  <si>
+    <t>AzureStorage</t>
+  </si>
+  <si>
+    <t>EntityFramework</t>
+  </si>
+  <si>
+    <t>EntityFrameworkCore</t>
+  </si>
+  <si>
+    <t>MailKit</t>
+  </si>
+  <si>
+    <t>RestSharp</t>
+  </si>
+  <si>
+    <t>SimpleInjector</t>
+  </si>
+  <si>
+    <t>ZXingNet</t>
+  </si>
+  <si>
+    <t>15.0.0</t>
   </si>
 </sst>
 </file>
@@ -624,9 +661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1059,4 +1096,483 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83531-2FF1-4980-A438-A4C479EB4D1B}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="12" width="18.17578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Made every method in the ObjectServiceAuditDecorator class virtual so that the class can be inherited and the methods overwritten. Enahnced the constructor to accept an ILogger instance and implemented appropriate logging. - Added the "class" contraint to the TContent generic parameter for Post and Put methods of the IRestClient interface. - Added an extension class for the ILogger interface. - Updated the RestSharpClient and NewtonsoftJsonDeserializer classes due to backward incompatibility issues with the upgrade of the RestSharp NuGet package. - Updated third-party NuGet packages. - Dropped .NET 5 and .NET Framework 4.7.2 as targeted frameworks for the following projects:   - Framework   - Framework.AuditNET   - Framework.AzureStorage   - Framework.MailKit   - Framework.RestSharp   - Framework.SimpleInjector   - Framework.ZXingNet
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A438A738-780C-40C4-B417-C1F3BF3F7837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5381D53-3B6F-4FA9-90EA-4132E8A7CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tardigrade" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Versions" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,34 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="99">
-  <si>
-    <t>Tardigrade.Framework</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.AspNet</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.AspNetCore</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.AuditNET</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.AzureStorage</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.EntityFramework</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.EntityFrameworkCore</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.RestSharp</t>
-  </si>
-  <si>
-    <t>Tardigrade.Framework.SimpleInjector</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
   <si>
     <t>10.4.0</t>
   </si>
@@ -142,9 +114,6 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>Tardigrade.Framework.ZXingNet</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -283,9 +252,6 @@
     <t>8.0.0</t>
   </si>
   <si>
-    <t>Tardigrade.Framework.MailKit</t>
-  </si>
-  <si>
     <t>14.1.0</t>
   </si>
   <si>
@@ -323,6 +289,15 @@
   </si>
   <si>
     <t>15.0.0</t>
+  </si>
+  <si>
+    <t>16.0.0</t>
+  </si>
+  <si>
+    <t>6.0.1</t>
+  </si>
+  <si>
+    <t>12.0.1</t>
   </si>
 </sst>
 </file>
@@ -658,453 +633,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:O12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <cols>
-    <col min="1" max="1" width="38.52734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K2" t="s">
-        <v>74</v>
-      </c>
-      <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="N3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
-      </c>
-      <c r="N5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="N6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="N10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="N11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="N12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83531-2FF1-4980-A438-A4C479EB4D1B}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1114,206 +648,206 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="F6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1321,16 +855,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -1338,55 +872,55 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -1394,64 +928,64 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1459,24 +993,24 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1484,91 +1018,129 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>83</v>
-      </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
         <v>37</v>
       </c>
-      <c r="J14" t="s">
-        <v>47</v>
-      </c>
       <c r="K14" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L14" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F16" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H16" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+      <c r="J16" t="s">
         <v>73</v>
       </c>
-      <c r="I16" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" t="s">
-        <v>83</v>
-      </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" t="s">
+        <v>90</v>
+      </c>
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated ObjectServiceAuditDecorator.cs to better support inheritance. - Updated ApplicationConfiguraton.cs to make support of User Secrets more intuitive. - Added a new test project for Tardigrade.Framework.AuditNET. - Set the <Nulable> property for all .NET 6 SDK-style test projects to "enable" and refactored code where appropriate.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5381D53-3B6F-4FA9-90EA-4132E8A7CC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D30B2-3E56-4F52-A6FD-CEEDAB43E038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="55020" yWindow="3240" windowWidth="16188" windowHeight="10068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
   <si>
     <t>10.4.0</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>12.0.1</t>
+  </si>
+  <si>
+    <t>17.0.0</t>
   </si>
 </sst>
 </file>
@@ -634,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83531-2FF1-4980-A438-A4C479EB4D1B}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1143,6 +1146,17 @@
         <v>70</v>
       </c>
     </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
- Added an Azure Storage specific application configuration class. - Added unit tests for the audit decorator. - Updated third-party NuGet packages. - Code clean-up.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D30B2-3E56-4F52-A6FD-CEEDAB43E038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F00E8F-7AC3-4A7A-8412-92EBA90B1713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55020" yWindow="3240" windowWidth="16188" windowHeight="10068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2853" yWindow="973" windowWidth="19954" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
   <si>
     <t>10.4.0</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>17.0.0</t>
+  </si>
+  <si>
+    <t>6.0.2</t>
   </si>
 </sst>
 </file>
@@ -641,7 +644,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1153,8 +1156,17 @@
       <c r="B18" t="s">
         <v>87</v>
       </c>
+      <c r="D18" t="s">
+        <v>92</v>
+      </c>
       <c r="E18" t="s">
         <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Moved the AzureQueueDataProvider.cs class from TikForce.Framework.AuditNET project to the newly added TikForce.Framework.AuditNET.AzureStorageQueue project. Refactored references accordingly. - Upgraded the AzureQueueDataProvider.cs class to use the Azure.Storage.Queues package instead of the deprecated Microsoft.Azure.Storage.Queue package. Updated the code accordingly.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F00E8F-7AC3-4A7A-8412-92EBA90B1713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B949DB0B-841E-42E9-943E-1DDDC3F95A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2853" yWindow="973" windowWidth="19954" windowHeight="10067" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>10.4.0</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>6.0.2</t>
+  </si>
+  <si>
+    <t>AuditNET.AzureStorage.Queue</t>
   </si>
 </sst>
 </file>
@@ -640,19 +643,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83531-2FF1-4980-A438-A4C479EB4D1B}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="12" width="18.17578125" customWidth="1"/>
+    <col min="1" max="5" width="18.17578125" customWidth="1"/>
+    <col min="6" max="6" width="26.05859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="18.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -669,28 +674,31 @@
         <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -707,28 +715,31 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,29 +755,32 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -782,29 +796,32 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -820,63 +837,72 @@
       <c r="E5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -892,47 +918,53 @@
       <c r="E8" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -948,29 +980,32 @@
       <c r="E10" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -983,21 +1018,24 @@
       <c r="D11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1008,32 +1046,38 @@
       <c r="D12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="F13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -1050,36 +1094,42 @@
         <v>73</v>
       </c>
       <c r="F14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" t="s">
         <v>74</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>63</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>28</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>37</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>70</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -1093,25 +1143,28 @@
         <v>70</v>
       </c>
       <c r="F16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>63</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>37</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>73</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>32</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -1128,28 +1181,31 @@
         <v>32</v>
       </c>
       <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
         <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>90</v>
       </c>
       <c r="H17" t="s">
         <v>90</v>
       </c>
       <c r="I17" t="s">
+        <v>90</v>
+      </c>
+      <c r="J17" t="s">
         <v>73</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>70</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>38</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -1160,12 +1216,15 @@
         <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
         <v>64</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
General code clean up.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B949DB0B-841E-42E9-943E-1DDDC3F95A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14590DCA-134E-4D6E-9A0B-E42F809957D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
   <si>
     <t>10.4.0</t>
   </si>
@@ -647,7 +647,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1227,6 +1227,9 @@
       <c r="I18" t="s">
         <v>65</v>
       </c>
+      <c r="L18" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Made the DbHelper.GenerateCreateScript() method into an extension method of the DbContextExtension.cs class. - Properly implemented the IDisposable pattern in the UnitTestClassFixture.cs class. - Created the EntityFrameworkCoreClassFixture.cs class that the extends UnitTestClassFixture.cs class from the Tardigrade.Framework project. Refactored the BlogTest.cs and UserTest.cs classes to use this new class fixture. - Deleted the deprecated DateTimeJsonConverter.cs and NewtonsoftJsonExtension.cs classes from the Tardigrade.Shared.Tests project.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capta\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC918E6-C176-46BE-83BB-A8379F4C308C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF8C37C-631A-408F-BBF4-0549F0E6E1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="3" r:id="rId1"/>
@@ -642,19 +642,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F83531-2FF1-4980-A438-A4C479EB4D1B}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L19" sqref="L19"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="5" width="18.17578125" customWidth="1"/>
-    <col min="6" max="6" width="26.05859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="18.17578125" customWidth="1"/>
+    <col min="1" max="5" width="18.19921875" customWidth="1"/>
+    <col min="6" max="6" width="26.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="18.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -695,7 +695,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,7 +736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +777,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -818,7 +818,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -859,7 +859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -879,7 +879,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -899,7 +899,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -940,7 +940,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -961,7 +961,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1032,7 +1032,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1060,7 +1060,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -1202,7 +1202,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>64</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="L18" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Updated project version numbers.
</commit_message>
<xml_diff>
--- a/Project version numbers.xlsx
+++ b/Project version numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\capta\Source\tardigrade-framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafidzalRafiq\Source\tardigrade-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF8C37C-631A-408F-BBF4-0549F0E6E1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D255326-4735-4DF9-9C13-B0FB6454BFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11422" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
   <si>
     <t>10.4.0</t>
   </si>
@@ -303,7 +303,22 @@
     <t>17.0.0</t>
   </si>
   <si>
-    <t>AuditNET.AzureStorage.Queue</t>
+    <t>4.1.0</t>
+  </si>
+  <si>
+    <t>6.0.2</t>
+  </si>
+  <si>
+    <t>AuditNET.AzureStorageQueue</t>
+  </si>
+  <si>
+    <t>12.0.2</t>
+  </si>
+  <si>
+    <t>3.0.1</t>
+  </si>
+  <si>
+    <t>4.0.1</t>
   </si>
 </sst>
 </file>
@@ -644,17 +659,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="5" width="18.19921875" customWidth="1"/>
-    <col min="6" max="6" width="26.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="13" width="18.19921875" customWidth="1"/>
+    <col min="1" max="5" width="18.17578125" customWidth="1"/>
+    <col min="6" max="6" width="26.05859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="13" width="18.17578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -671,7 +686,7 @@
         <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>80</v>
@@ -695,7 +710,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -736,7 +751,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +792,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -818,7 +833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -859,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -879,7 +894,7 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -899,7 +914,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>43</v>
       </c>
@@ -940,7 +955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -961,7 +976,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
@@ -1002,7 +1017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1032,7 +1047,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1060,7 +1075,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
@@ -1074,7 +1089,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>72</v>
       </c>
@@ -1115,7 +1130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -1126,7 +1141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -1202,13 +1217,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B18" t="s">
         <v>87</v>
       </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
@@ -1221,11 +1239,23 @@
       <c r="G18" t="s">
         <v>64</v>
       </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
       <c r="I18" t="s">
         <v>69</v>
       </c>
+      <c r="J18" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" t="s">
+        <v>92</v>
+      </c>
       <c r="L18" t="s">
         <v>42</v>
+      </c>
+      <c r="M18" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>